<commit_message>
added daty dodania ogloszen
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,61 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kub\Documents\VSCodeProjects\jobscrapper\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E99D455-BC72-4E5C-87EC-1A4AC041F717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet_name_3" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet_name_3" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -78,32 +72,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -391,110 +453,503 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C24" sqref="A1:C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D1:D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="73.42578125" customWidth="1"/>
-    <col min="3" max="3" width="209.7109375" customWidth="1"/>
+    <col width="73.42578125" customWidth="1" min="2" max="2"/>
+    <col width="18.140625" customWidth="1" min="3" max="3"/>
+    <col width="199.5703125" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="C23" s="1"/>
+    <row r="1">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>oferty</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>daty</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>linki</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Threat Intelligence Engineer Internship</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>17 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/threat-intelligence-engineer-internship-warszawa-plac-europejski-1,oferta,1004449987?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy&amp;ref=top_boosterAI_L2_1_1_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Analityk w Zespole IT</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>18 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/analityk-w-zespole-it-warszawa-ksiazeca-4,oferta,1004461967?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Asystent / Asystentka ds. helpdesk</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>18 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/asystent-asystentka-ds-helpdesk-warszawa,oferta,1004486715?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Kundenservice-Mitarbeiter (1st Level Support)</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>18 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D5" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/kundenservice-mitarbeiter-1st-level-support-warszawa,oferta,1004485749?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Staż w Dziale HelpDesk</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>18 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D6" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/staz-w-dziale-helpdesk-warszawa-domaniewska-49,oferta,1004485275?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Asystent / Asystentka ds. Helpdesk</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>17 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D7" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/asystent-asystentka-ds-helpdesk-warszawa-wiertnicza-126,oferta,1004483969?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Płatne praktyki | Data Governance</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>17 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D8" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/platne-praktyki-data-governance-warszawa-polna-11,oferta,1004433654?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Program Stażowy – Crypto Algorithmic Trader 2026</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>17 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D9" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/program-stazowy-crypto-algorithmic-trader-2026-warszawa-gieldowa-5,oferta,1004454995?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Threat Intelligence Engineer Internship</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>17 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/threat-intelligence-engineer-internship-warszawa-plac-europejski-1,oferta,1004449987?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>DevOps Academy Program</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>17 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/devops-academy-program-warszawa-twarda-18,oferta,1004447202?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>IT &amp; Data DanONE Internship in Global Data &amp; Analytics Team</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>16 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/it-data-danone-internship-in-global-data-analytics-team-warszawa-bobrowiecka-8,oferta,1004466484?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Płatny staż – Administrator IT (k/m)</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>16 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/platny-staz-administrator-it-k-m-warszawa-jutrzenki-105,oferta,1004463345?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SAP Intern</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>15 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D14" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/sap-intern-warszawa-zwirki-i-wigury-16a,oferta,1004453786?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Junior Helpdesk Specialist</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="inlineStr">
+        <is>
+          <t>15 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D15" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/junior-helpdesk-specialist-warszawa-aleja-jana-pawla-ii-22,oferta,1004471006?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Fabryka Talentów - Program Stażowy w Analityce Danych (Komórka Logistyki)</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>14 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/fabryka-talentow-program-stazowy-w-analityce-danych-komorka-logistyki-kanie-pow-pruszkowski-warszawska-21,oferta,1004480295?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Junior IT Administrator (Intern)</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>14 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D17" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/junior-it-administrator-intern-warszawa-aleje-jerozolimskie-181a,oferta,1004460218?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Student/Studentka do Działu IT</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>14 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/student-studentka-do-dzialu-it-warszawa-swietokrzyska-14,oferta,1004475706?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Paid Internship in IT - Low-Code/No-Code Development (f/m)</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="inlineStr">
+        <is>
+          <t>13 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D19" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/paid-internship-in-it-low-code-no-code-development-f-m-warszawa-jutrzenki-105,oferta,1004447570?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Młodszy Programista Python – staż w dziale DOK</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>12 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/mlodszy-programista-python-staz-w-dziale-dok-pruszkow-przejazdowa-22,oferta,1004449633?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Asystent IT (k/m)</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>12 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D21" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/asystent-it-k-m-blonie,oferta,1004444801?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Młodszy/a konsultant/ka Service Desk</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>11 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/mlodszy-a-konsultant-ka-service-desk-warszawa-plac-konesera-12,oferta,1004439157?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Solutions Architect Intern</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="inlineStr">
+        <is>
+          <t>7 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D23" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/solutions-architect-intern-warszawa,oferta,1004465641?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Stażysta w Zespole Systemów Ubezpieczeń Majątkowych (f/m/d)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>6 listopada 2025</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>https://www.pracuj.pl/praca/stazysta-w-zespole-systemow-ubezpieczen-majatkowych-f-m-d-warszawa-inflancka-4,oferta,1004430318?s=6a3a7038&amp;searchId=MTc2MzQ5NjUwMzc2MC4wNzQy</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>